<commit_message>
Add Lab #1 Changes
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Enable NIC Teaming adapters 0 &amp; 1</t>
   </si>
   <si>
-    <t>Seconds</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -75,6 +72,30 @@
   </si>
   <si>
     <t>Evan</t>
+  </si>
+  <si>
+    <t>Online &amp; Initialize Disks 1-4</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Create Spanned Volume on Disks 1-4</t>
+  </si>
+  <si>
+    <t>Create Mirrored Volume on Disks 1&amp;2</t>
+  </si>
+  <si>
+    <t>Create RAID-5 Volume Disks 1-4</t>
+  </si>
+  <si>
+    <t>Create Mounted Volume @ C:/Mount</t>
   </si>
 </sst>
 </file>
@@ -168,10 +189,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +500,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,14 +515,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -513,7 +534,9 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
@@ -545,70 +568,142 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>42754</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="F5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>42754</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="A7" s="7">
+        <v>42754</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="A8" s="7">
+        <v>42754</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="7">
+        <v>42754</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="7">
+        <v>42754</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>

</xml_diff>

<commit_message>
Update Server log for Lab 3 Complete Project 1 Server Editions
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -96,6 +96,27 @@
   </si>
   <si>
     <t>Create Mounted Volume @ C:/Mount</t>
+  </si>
+  <si>
+    <t>Remove NIC Team 1</t>
+  </si>
+  <si>
+    <t>Set Eth1 Static IP 10.130.26.131</t>
+  </si>
+  <si>
+    <t>Install Roles (AD DS, DHCP, DNS, IIS, Print)</t>
+  </si>
+  <si>
+    <t>Remove Print Roles</t>
+  </si>
+  <si>
+    <t>Enable roles</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Seconds</t>
   </si>
 </sst>
 </file>
@@ -499,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,52 +727,122 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="7">
+        <v>42759</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="7">
+        <v>42759</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="A13" s="7">
+        <v>42759</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="A14" s="7">
+        <v>42759</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="7">
+        <v>42759</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>

</xml_diff>

<commit_message>
Begin Lab 4 Updates Evan Schober Server Log.xlsx
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="85">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -274,6 +274,9 @@
   <si>
     <t>wpots</t>
   </si>
+  <si>
+    <t>Limit Borey Chan login hours (bchan)</t>
+  </si>
 </sst>
 </file>
 
@@ -367,11 +370,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +683,7 @@
   <dimension ref="A1:G830"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,14 +698,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1027,7 +1030,7 @@
       <c r="A17" s="7">
         <v>42766</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1073,7 +1076,7 @@
       <c r="A19" s="7">
         <v>42766</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -1119,7 +1122,7 @@
       <c r="A21" s="7">
         <v>42766</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1165,7 +1168,7 @@
       <c r="A23" s="7">
         <v>42766</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1211,7 +1214,7 @@
       <c r="A25" s="7">
         <v>42766</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1280,7 +1283,7 @@
       <c r="A28" s="7">
         <v>42766</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -1760,13 +1763,27 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+      <c r="A49" s="7">
+        <v>42768</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>

</xml_diff>

<commit_message>
Update "Evan Schober Server Log.xlsx" for Lab 5
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="96">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -276,6 +276,39 @@
   </si>
   <si>
     <t>Limit Borey Chan login hours (bchan)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Create Sales Laptops 1,2,3</t>
+  </si>
+  <si>
+    <t>Create Sales Workstations 1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>Create Marketing Workstations 1,2,3</t>
+  </si>
+  <si>
+    <t>Create Marketing Laptops 1,2,3</t>
+  </si>
+  <si>
+    <t>Create Accounting Workstations 1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>Create Accounting Laptops 1,2</t>
+  </si>
+  <si>
+    <t>Create Admins Workstations 1,2,3</t>
+  </si>
+  <si>
+    <t>Create Admins Laptops 1,2,3</t>
+  </si>
+  <si>
+    <t>Create Research Workstations 1,2,3,4</t>
+  </si>
+  <si>
+    <t>Create Support Workstations</t>
   </si>
 </sst>
 </file>
@@ -682,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,94 +1819,234 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="A50" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="A51" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="A52" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="A53" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
+      <c r="A54" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
+      <c r="A55" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
+      <c r="A56" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="A57" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="A58" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
+      <c r="A59" s="7">
+        <v>42775</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>

</xml_diff>

<commit_message>
Update Evan Schober Server Log.xlsx for Lab 8
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="137">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -393,6 +393,45 @@
   </si>
   <si>
     <t>jrons, tplask, semery</t>
+  </si>
+  <si>
+    <t>Create Managers distribution group</t>
+  </si>
+  <si>
+    <t>Add Accounting managers to Managers group</t>
+  </si>
+  <si>
+    <t>Add Marketing managers to Managers group</t>
+  </si>
+  <si>
+    <t>Add Research-Dev managers to Managers group</t>
+  </si>
+  <si>
+    <t>Add Sales managers to Managers group</t>
+  </si>
+  <si>
+    <t>Add Support managers to Managers group</t>
+  </si>
+  <si>
+    <t>Create Support Resources group</t>
+  </si>
+  <si>
+    <t>Add Support group to Support Resources group</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Delegate control of adding computers to the Domain to ComputerAdmins group</t>
+  </si>
+  <si>
+    <t>Delegate control of domain PW Resets to PasswordAdmins group</t>
+  </si>
+  <si>
+    <t>Delegate control of departmental OUs to GPOLinkAdmins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounting,Marketing, Research-Dev, Sales, &amp; Support OUs </t>
   </si>
 </sst>
 </file>
@@ -552,20 +591,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,6 +608,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,14 +940,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -926,36 +965,36 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>42754</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -978,7 +1017,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>42754</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1001,7 +1040,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>42754</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1024,7 +1063,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>42754</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1047,7 +1086,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>42754</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1070,7 +1109,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>42754</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1093,7 +1132,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>42759</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1116,7 +1155,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>42759</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1139,7 +1178,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>42759</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1162,7 +1201,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>42759</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1185,7 +1224,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>42759</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1208,7 +1247,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>42766</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1231,7 +1270,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>42766</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1254,7 +1293,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>42766</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1277,7 +1316,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>42766</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1300,7 +1339,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>42766</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1323,7 +1362,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>42766</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1346,7 +1385,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="7">
         <v>42766</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1369,7 +1408,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="7">
         <v>42766</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1392,7 +1431,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="7">
         <v>42766</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1415,7 +1454,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="7">
         <v>42766</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1438,7 +1477,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="7">
         <v>42766</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1461,7 +1500,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="7">
         <v>42766</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1484,7 +1523,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="7">
         <v>42766</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1507,7 +1546,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="7">
         <v>42766</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1530,7 +1569,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="7">
         <v>42766</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1553,7 +1592,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="7">
         <v>42766</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1576,7 +1615,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="7">
         <v>42766</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1599,7 +1638,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="7">
         <v>42766</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1622,7 +1661,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="7">
         <v>42766</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1645,7 +1684,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="7">
         <v>42766</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1668,7 +1707,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="7">
         <v>42766</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1691,7 +1730,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+      <c r="A37" s="7">
         <v>42766</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1714,7 +1753,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="7">
         <v>42766</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1737,7 +1776,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="7">
         <v>42766</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1760,7 +1799,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="A40" s="7">
         <v>42766</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1783,7 +1822,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+      <c r="A41" s="7">
         <v>42766</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -1806,7 +1845,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+      <c r="A42" s="7">
         <v>42766</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1829,7 +1868,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+      <c r="A43" s="7">
         <v>42766</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -1852,7 +1891,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
+      <c r="A44" s="7">
         <v>42766</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -1875,7 +1914,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
+      <c r="A45" s="7">
         <v>42766</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -1898,7 +1937,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+      <c r="A46" s="7">
         <v>42766</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1921,7 +1960,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+      <c r="A47" s="7">
         <v>42766</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -1944,7 +1983,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
+      <c r="A48" s="7">
         <v>42766</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -1967,7 +2006,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
+      <c r="A49" s="7">
         <v>42768</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1990,7 +2029,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
+      <c r="A50" s="7">
         <v>42775</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -2013,7 +2052,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
+      <c r="A51" s="7">
         <v>42775</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -2036,7 +2075,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
+      <c r="A52" s="7">
         <v>42775</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2059,7 +2098,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="8">
+      <c r="A53" s="7">
         <v>42775</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -2082,7 +2121,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
+      <c r="A54" s="7">
         <v>42775</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -2105,7 +2144,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="8">
+      <c r="A55" s="7">
         <v>42775</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -2128,7 +2167,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="8">
+      <c r="A56" s="7">
         <v>42775</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -2151,7 +2190,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="8">
+      <c r="A57" s="7">
         <v>42775</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -2174,7 +2213,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
+      <c r="A58" s="7">
         <v>42775</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -2197,7 +2236,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
+      <c r="A59" s="7">
         <v>42775</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -2220,7 +2259,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="8">
+      <c r="A60" s="7">
         <v>42782</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -2243,7 +2282,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="8">
+      <c r="A61" s="7">
         <v>42787</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -2266,7 +2305,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8">
+      <c r="A62" s="7">
         <v>42787</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -2289,7 +2328,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
+      <c r="A63" s="7">
         <v>42787</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -2312,7 +2351,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="8">
+      <c r="A64" s="7">
         <v>42787</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -2335,7 +2374,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="8">
+      <c r="A65" s="7">
         <v>42787</v>
       </c>
       <c r="B65" s="5" t="s">
@@ -2358,7 +2397,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
+      <c r="A66" s="7">
         <v>42787</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -2381,7 +2420,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="8">
+      <c r="A67" s="7">
         <v>42787</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -2404,7 +2443,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="8">
+      <c r="A68" s="7">
         <v>42787</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -2427,7 +2466,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="8">
+      <c r="A69" s="7">
         <v>42787</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -2450,7 +2489,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
+      <c r="A70" s="7">
         <v>42787</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -2473,7 +2512,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
+      <c r="A71" s="7">
         <v>42787</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -2496,7 +2535,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
+      <c r="A72" s="7">
         <v>42787</v>
       </c>
       <c r="B72" s="5" t="s">
@@ -2519,7 +2558,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="8">
+      <c r="A73" s="7">
         <v>42787</v>
       </c>
       <c r="B73" s="5" t="s">
@@ -2542,7 +2581,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
+      <c r="A74" s="7">
         <v>42787</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -2565,7 +2604,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="8">
+      <c r="A75" s="7">
         <v>42787</v>
       </c>
       <c r="B75" s="5" t="s">
@@ -2588,7 +2627,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+      <c r="A76" s="7">
         <v>42787</v>
       </c>
       <c r="B76" s="5" t="s">
@@ -2611,7 +2650,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="8">
+      <c r="A77" s="7">
         <v>42787</v>
       </c>
       <c r="B77" s="5" t="s">
@@ -2629,12 +2668,12 @@
       <c r="F77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G77" s="13" t="s">
+      <c r="G77" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+      <c r="A78" s="7">
         <v>42787</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -2649,16 +2688,16 @@
       <c r="E78" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F78" s="11" t="s">
+      <c r="F78" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H78" s="12"/>
+      <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
+      <c r="A79" s="7">
         <v>42787</v>
       </c>
       <c r="B79" s="5" t="s">
@@ -2676,108 +2715,262 @@
       <c r="F79" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="G79" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
+      <c r="A80" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
+      <c r="A81" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
+      <c r="A82" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
+      <c r="A84" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
+      <c r="A85" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
+      <c r="A86" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
+      <c r="A87" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
+        <v>42796</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>

</xml_diff>

<commit_message>
Update Evan Schober Server Log.xlsx for Lab 9
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="163">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -432,6 +432,84 @@
   </si>
   <si>
     <t xml:space="preserve">Accounting,Marketing, Research-Dev, Sales, &amp; Support OUs </t>
+  </si>
+  <si>
+    <t>Create Accounting Resources group</t>
+  </si>
+  <si>
+    <t>Add Accounting group to accounting resources group</t>
+  </si>
+  <si>
+    <t>Create Research Resources group</t>
+  </si>
+  <si>
+    <t>Add Research-Dev group to Research Resources group</t>
+  </si>
+  <si>
+    <t>Create Sales Resources domain group</t>
+  </si>
+  <si>
+    <t>Add Sales group to Sales Resources group</t>
+  </si>
+  <si>
+    <t>Create Departments, Personnel &amp; Finances folders</t>
+  </si>
+  <si>
+    <t>Create departmental folders Accounting,Research,Sales, &amp; Support within Departments folder</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Research-Dev</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Share Personnel &amp; Finances folders</t>
+  </si>
+  <si>
+    <t>Share Accounting folder, Set Accounting Resources NTFS Permissions "Full Control"</t>
+  </si>
+  <si>
+    <t>Share Research folder, Set Research Resources NTFS Permissions "Full Control"</t>
+  </si>
+  <si>
+    <t>Share Sales folder, Set Sales Resources NTFS Permissions "Full Control"</t>
+  </si>
+  <si>
+    <t>Share Support folder, Set Support Resources NTFS Permissions "Full Control"</t>
+  </si>
+  <si>
+    <t>Change Managers Domain Distribution group to Global Security</t>
+  </si>
+  <si>
+    <t>Managers</t>
+  </si>
+  <si>
+    <t>Set Personnel NTFS File permissions to "Full Control" by Managers group, Removed inherited permissions</t>
+  </si>
+  <si>
+    <t>Create shared folders Projects, Shared, Archives, Confidential, &amp; Components</t>
+  </si>
+  <si>
+    <t>Share Users folder with names Users &amp; Home</t>
+  </si>
+  <si>
+    <t>Enable caching of Archives folder &amp; Optimize for performance</t>
+  </si>
+  <si>
+    <t>Disable caching of Confidential shared folder</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Grant Users group Modify and Write access to Shared folder in NTFS permissions</t>
   </si>
 </sst>
 </file>
@@ -922,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H830"/>
+  <dimension ref="A1:H838"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,184 +3051,462 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="A91" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
+      <c r="A93" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
+      <c r="A95" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
+      <c r="A96" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
+      <c r="A98" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="5"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="5"/>
+      <c r="A107" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
+      <c r="A109" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="7">
+        <v>42808</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
@@ -9631,6 +9987,77 @@
       <c r="E830" s="5"/>
       <c r="F830" s="5"/>
       <c r="G830" s="5"/>
+    </row>
+    <row r="831" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A831" s="5"/>
+      <c r="B831" s="5"/>
+      <c r="C831" s="5"/>
+      <c r="D831" s="5"/>
+      <c r="E831" s="5"/>
+      <c r="F831" s="5"/>
+      <c r="G831" s="5"/>
+    </row>
+    <row r="832" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A832" s="5"/>
+      <c r="B832" s="5"/>
+      <c r="C832" s="5"/>
+      <c r="D832" s="5"/>
+      <c r="E832" s="5"/>
+      <c r="F832" s="5"/>
+      <c r="G832" s="5"/>
+    </row>
+    <row r="833" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A833" s="5"/>
+      <c r="B833" s="5"/>
+      <c r="C833" s="5"/>
+      <c r="D833" s="5"/>
+      <c r="E833" s="5"/>
+      <c r="F833" s="5"/>
+      <c r="G833" s="5"/>
+    </row>
+    <row r="834" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A834" s="5"/>
+      <c r="B834" s="5"/>
+      <c r="C834" s="5"/>
+      <c r="D834" s="5"/>
+      <c r="E834" s="5"/>
+      <c r="F834" s="5"/>
+      <c r="G834" s="5"/>
+    </row>
+    <row r="835" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A835" s="5"/>
+      <c r="B835" s="5"/>
+      <c r="C835" s="5"/>
+      <c r="D835" s="5"/>
+      <c r="E835" s="5"/>
+      <c r="F835" s="5"/>
+      <c r="G835" s="5"/>
+    </row>
+    <row r="836" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A836" s="5"/>
+      <c r="B836" s="5"/>
+      <c r="C836" s="5"/>
+      <c r="D836" s="5"/>
+      <c r="E836" s="5"/>
+      <c r="F836" s="5"/>
+      <c r="G836" s="5"/>
+    </row>
+    <row r="837" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A837" s="5"/>
+      <c r="B837" s="5"/>
+      <c r="C837" s="5"/>
+      <c r="D837" s="5"/>
+      <c r="E837" s="5"/>
+      <c r="F837" s="5"/>
+      <c r="G837" s="5"/>
+    </row>
+    <row r="838" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B838" s="5"/>
+      <c r="C838" s="5"/>
+      <c r="D838" s="5"/>
+      <c r="E838" s="5"/>
+      <c r="F838" s="5"/>
+      <c r="G838" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update Evan Schober Server Log.xlsx for Lab 11
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="191">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -510,6 +510,90 @@
   </si>
   <si>
     <t>Grant Users group Modify and Write access to Shared folder in NTFS permissions</t>
+  </si>
+  <si>
+    <t>Create Workstation Settings GPO</t>
+  </si>
+  <si>
+    <t>Add cis to Domain Admins Group</t>
+  </si>
+  <si>
+    <t>cis</t>
+  </si>
+  <si>
+    <t>Link OU's to Workstation Settings GPO</t>
+  </si>
+  <si>
+    <t>TempMarketing, TempSales, Support</t>
+  </si>
+  <si>
+    <t>Configure Default Password Policy</t>
+  </si>
+  <si>
+    <t>Enable auditing of logon attempts within Accounting GPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure Accounting Event Log Settings: Do not overwrite events. </t>
+  </si>
+  <si>
+    <t>Enable Accounting Audit security options. Shut down computer if unable to log events</t>
+  </si>
+  <si>
+    <t>Configure Default Domain GPO: Disable guest account, Do not display last user name, Disable anynomous name translation, Disable anon. enumeration of SAM accounts, Disable anon. enum. Of SAM accounts &amp; shares.</t>
+  </si>
+  <si>
+    <t>Create Accounting GPO</t>
+  </si>
+  <si>
+    <t>Create Support GPO</t>
+  </si>
+  <si>
+    <t>Disable Support GPO User Configuration</t>
+  </si>
+  <si>
+    <t>Configure Support GPO: Disable cached logons, Require DC authentication, Force logoff when logon hours expire, Allow shutdown w/o logon</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Enable admin approval for built in Admin account</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Disable UIAccess applications to prompt for elevation without using the secure desktop</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Set Admin Approval elevation prompt to Prompt for credentials</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Automatically deny elevation requests from standard users</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Promp for elevation when an installation is detected</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Elevate all executables regardless of signature and validation status</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Only elevate UI apps installed in secure locations</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Run all admins in Admin Approval mode</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Switch to secure desktop when prompting for elevation</t>
+  </si>
+  <si>
+    <t>Configure User Account Control: Virtualize file and registry write failures to per user locations</t>
+  </si>
+  <si>
+    <t>Create Desktop Admins in Admins OU</t>
+  </si>
+  <si>
+    <t>Add Admins to Desktop Admins</t>
+  </si>
+  <si>
+    <t>eschober, jgolden, sbarnes</t>
+  </si>
+  <si>
+    <t>Create Workstations GPO</t>
   </si>
 </sst>
 </file>
@@ -549,7 +633,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -652,11 +736,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,6 +791,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H838"/>
+  <dimension ref="A1:H839"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3509,229 +3610,569 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="5"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5"/>
+      <c r="A111" s="15">
+        <v>42829</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C111" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E111" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="F111" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
+      <c r="A112" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
+      <c r="A114" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
+      <c r="A115" s="18">
+        <v>42829</v>
+      </c>
+      <c r="B115" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C115" s="17"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="17"/>
+      <c r="G115" s="17"/>
+    </row>
+    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A119" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="5"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
+      <c r="A120" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="5"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
-      <c r="G124" s="5"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="5"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="5"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="5"/>
-      <c r="B127" s="5"/>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="5"/>
-      <c r="G127" s="5"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="5"/>
-      <c r="B128" s="5"/>
-      <c r="C128" s="5"/>
-      <c r="D128" s="5"/>
-      <c r="E128" s="5"/>
-      <c r="F128" s="5"/>
-      <c r="G128" s="5"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="5"/>
-      <c r="B129" s="5"/>
-      <c r="C129" s="5"/>
-      <c r="D129" s="5"/>
-      <c r="E129" s="5"/>
-      <c r="F129" s="5"/>
-      <c r="G129" s="5"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="5"/>
-      <c r="B130" s="5"/>
-      <c r="C130" s="5"/>
-      <c r="D130" s="5"/>
-      <c r="E130" s="5"/>
-      <c r="F130" s="5"/>
-      <c r="G130" s="5"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="5"/>
-      <c r="B131" s="5"/>
-      <c r="C131" s="5"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
-      <c r="G131" s="5"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
-      <c r="B132" s="5"/>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
-      <c r="G132" s="5"/>
+      <c r="A121" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A122" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A128" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
-      <c r="G133" s="5"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="5"/>
-      <c r="B134" s="5"/>
-      <c r="C134" s="5"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5"/>
+      <c r="A133" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="5"/>
-      <c r="B135" s="5"/>
-      <c r="C135" s="5"/>
-      <c r="D135" s="5"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="5"/>
-      <c r="G135" s="5"/>
+      <c r="A135" s="7">
+        <v>42829</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G135" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
@@ -10052,12 +10493,21 @@
       <c r="G837" s="5"/>
     </row>
     <row r="838" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A838" s="5"/>
       <c r="B838" s="5"/>
       <c r="C838" s="5"/>
       <c r="D838" s="5"/>
       <c r="E838" s="5"/>
       <c r="F838" s="5"/>
       <c r="G838" s="5"/>
+    </row>
+    <row r="839" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B839" s="5"/>
+      <c r="C839" s="5"/>
+      <c r="D839" s="5"/>
+      <c r="E839" s="5"/>
+      <c r="F839" s="5"/>
+      <c r="G839" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update Evan Schober Server Log.xlsx for end of Lab 11
</commit_message>
<xml_diff>
--- a/Evan Schober Server Log.xlsx
+++ b/Evan Schober Server Log.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CIS223\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="150" windowWidth="14355" windowHeight="7995"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="193">
   <si>
     <t>CIS 232 Server Log</t>
   </si>
@@ -594,12 +589,18 @@
   </si>
   <si>
     <t>Create Workstations GPO</t>
+  </si>
+  <si>
+    <t>Desktop Admins</t>
+  </si>
+  <si>
+    <t>Add Desktop Admins to Workstations local Administrators group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -782,6 +783,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,12 +798,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,7 +858,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -892,7 +893,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1104,7 +1105,7 @@
   <dimension ref="A1:H839"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="H135" sqref="H135"/>
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,14 +1120,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1144,10 +1145,10 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -3610,25 +3611,25 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="15">
+      <c r="A111" s="12">
         <v>42829</v>
       </c>
-      <c r="B111" s="16" t="s">
+      <c r="B111" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C111" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E111" s="16" t="s">
+      <c r="C111" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E111" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F111" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G111" s="16" t="s">
+      <c r="F111" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3702,17 +3703,17 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="18">
+      <c r="A115" s="15">
         <v>42829</v>
       </c>
-      <c r="B115" s="17" t="s">
+      <c r="B115" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="G115" s="17"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
     </row>
     <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
@@ -4174,14 +4175,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="5"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="5"/>
-      <c r="E136" s="5"/>
-      <c r="F136" s="5"/>
-      <c r="G136" s="5"/>
+    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="7">
+        <v>42830</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>

</xml_diff>